<commit_message>
Update LMT with stock statistics.
</commit_message>
<xml_diff>
--- a/LMT/LMT.xlsx
+++ b/LMT/LMT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534a1defcf7f9d1a/Company Models CloudSave/LMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1257" documentId="11_8C59228DA9BE475EA05F70E42E9A2DC94B93B51C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7642071A-31A6-4B9A-A5BC-0D905238FC86}"/>
+  <xr:revisionPtr revIDLastSave="1383" documentId="11_8C59228DA9BE475EA05F70E42E9A2DC94B93B51C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70722108-268A-4A85-9CB1-4A5F15638D81}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5420" yWindow="2090" windowWidth="26720" windowHeight="17120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="2049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="2059">
   <si>
     <t>Ticker</t>
   </si>
@@ -6235,6 +6235,36 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Stock Statistics</t>
+  </si>
+  <si>
+    <t>Marketcap</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>P/FCF</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Revenue Growth</t>
+  </si>
+  <si>
+    <t>Earnings Growth</t>
+  </si>
+  <si>
+    <t>FCF Growth</t>
   </si>
 </sst>
 </file>
@@ -6366,7 +6396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6389,15 +6419,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6413,6 +6439,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7350,11 +7380,11 @@
   <dimension ref="B3:AM130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="N87" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="R100" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="B7" sqref="B7"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="S124" sqref="S124"/>
+      <selection pane="bottomRight" activeCell="Z131" sqref="Z131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7495,16 +7525,133 @@
       <c r="B7" t="s">
         <v>1965</v>
       </c>
+      <c r="S7">
+        <v>87.18</v>
+      </c>
+      <c r="T7">
+        <v>82.43</v>
+      </c>
+      <c r="U7">
+        <v>95.82</v>
+      </c>
+      <c r="V7">
+        <v>149.99</v>
+      </c>
+      <c r="W7">
+        <v>198.72</v>
+      </c>
+      <c r="X7">
+        <v>227.91</v>
+      </c>
+      <c r="Y7">
+        <v>269.89999999999998</v>
+      </c>
+      <c r="Z7">
+        <v>323.94</v>
+      </c>
+      <c r="AA7">
+        <v>363</v>
+      </c>
+      <c r="AB7">
+        <v>399.96</v>
+      </c>
+      <c r="AC7">
+        <v>442.53</v>
+      </c>
+      <c r="AD7">
+        <v>396.99</v>
+      </c>
+      <c r="AE7">
+        <v>498.95</v>
+      </c>
     </row>
     <row r="8" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>1966</v>
       </c>
+      <c r="S8">
+        <v>49.84</v>
+      </c>
+      <c r="T8">
+        <v>52.87</v>
+      </c>
+      <c r="U8">
+        <v>63.5</v>
+      </c>
+      <c r="V8">
+        <v>84.67</v>
+      </c>
+      <c r="W8">
+        <v>131.41</v>
+      </c>
+      <c r="X8">
+        <v>162.56</v>
+      </c>
+      <c r="Y8">
+        <v>196.58</v>
+      </c>
+      <c r="Z8">
+        <v>248</v>
+      </c>
+      <c r="AA8">
+        <v>241.18</v>
+      </c>
+      <c r="AB8">
+        <v>256.79000000000002</v>
+      </c>
+      <c r="AC8">
+        <v>266.11</v>
+      </c>
+      <c r="AD8">
+        <v>319.81</v>
+      </c>
+      <c r="AE8">
+        <v>353.03</v>
+      </c>
     </row>
     <row r="9" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>1967</v>
       </c>
+      <c r="S9">
+        <v>67.680000000000007</v>
+      </c>
+      <c r="T9">
+        <v>66.36</v>
+      </c>
+      <c r="U9">
+        <v>79.05</v>
+      </c>
+      <c r="V9">
+        <v>85.88</v>
+      </c>
+      <c r="W9">
+        <v>144.69</v>
+      </c>
+      <c r="X9">
+        <v>181.91</v>
+      </c>
+      <c r="Y9">
+        <v>200.47</v>
+      </c>
+      <c r="Z9">
+        <v>244.08</v>
+      </c>
+      <c r="AA9">
+        <v>279.98</v>
+      </c>
+      <c r="AB9">
+        <v>310.26</v>
+      </c>
+      <c r="AC9">
+        <v>347.56</v>
+      </c>
+      <c r="AD9">
+        <v>337.45</v>
+      </c>
+      <c r="AE9">
+        <v>417.73</v>
+      </c>
     </row>
     <row r="11" spans="2:39" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
@@ -9280,7 +9427,7 @@
       </c>
     </row>
     <row r="50" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="8" t="s">
         <v>438</v>
       </c>
       <c r="P50" s="8">
@@ -9381,7 +9528,7 @@
       </c>
     </row>
     <row r="51" spans="2:39" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="12" t="s">
         <v>769</v>
       </c>
       <c r="P51" s="12" t="e">
@@ -9487,7 +9634,7 @@
       </c>
     </row>
     <row r="53" spans="2:39" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="15" t="s">
         <v>1994</v>
       </c>
       <c r="S53" s="15">
@@ -9531,7 +9678,7 @@
       </c>
     </row>
     <row r="54" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="8" t="s">
         <v>569</v>
       </c>
       <c r="P54" s="8">
@@ -9632,7 +9779,7 @@
       </c>
     </row>
     <row r="55" spans="2:39" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="12" t="s">
         <v>1996</v>
       </c>
       <c r="P55" s="12" t="e">
@@ -9738,7 +9885,7 @@
       </c>
     </row>
     <row r="57" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="8" t="s">
         <v>2004</v>
       </c>
       <c r="S57" s="8">
@@ -9782,7 +9929,7 @@
       </c>
     </row>
     <row r="58" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="8" t="s">
         <v>2005</v>
       </c>
       <c r="S58" s="8">
@@ -9826,7 +9973,7 @@
       </c>
     </row>
     <row r="59" spans="2:39" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="15" t="s">
         <v>2006</v>
       </c>
       <c r="S59" s="15">
@@ -9870,7 +10017,7 @@
       </c>
     </row>
     <row r="60" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="8" t="s">
         <v>2007</v>
       </c>
       <c r="P60" s="8">
@@ -9971,7 +10118,7 @@
       </c>
     </row>
     <row r="61" spans="2:39" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="15" t="s">
         <v>2008</v>
       </c>
       <c r="S61" s="15">
@@ -10015,7 +10162,7 @@
       </c>
     </row>
     <row r="62" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="8" t="s">
         <v>2009</v>
       </c>
       <c r="P62" s="8">
@@ -10116,7 +10263,7 @@
       </c>
     </row>
     <row r="63" spans="2:39" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="15" t="s">
         <v>2010</v>
       </c>
       <c r="S63" s="15">
@@ -10160,7 +10307,7 @@
       </c>
     </row>
     <row r="64" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="8" t="s">
         <v>683</v>
       </c>
       <c r="P64" s="8">
@@ -10260,124 +10407,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="18"/>
-    </row>
-    <row r="66" spans="2:39" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="22" t="s">
+    <row r="65" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="19" t="s">
         <v>2011</v>
       </c>
-      <c r="P66" s="23" t="e">
+      <c r="P66" s="19" t="e">
         <f>P64/P67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q66" s="23" t="e">
+      <c r="Q66" s="19" t="e">
         <f t="shared" ref="Q66:AM66" si="37">Q64/Q67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R66" s="23" t="e">
+      <c r="R66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S66" s="23" t="e">
+      <c r="S66" s="19">
+        <f t="shared" si="37"/>
+        <v>8.2262651669977558</v>
+      </c>
+      <c r="T66" s="19">
+        <f t="shared" si="37"/>
+        <v>8.1665923317082161</v>
+      </c>
+      <c r="U66" s="19">
+        <f t="shared" si="37"/>
+        <v>8.5094378811034677</v>
+      </c>
+      <c r="V66" s="19">
+        <f t="shared" si="37"/>
+        <v>9.274181003639983</v>
+      </c>
+      <c r="W66" s="19">
+        <f t="shared" si="37"/>
+        <v>11.451820915575299</v>
+      </c>
+      <c r="X66" s="19">
+        <f t="shared" si="37"/>
+        <v>11.800829495199467</v>
+      </c>
+      <c r="Y66" s="19">
+        <f t="shared" si="37"/>
+        <v>17.818576373938654</v>
+      </c>
+      <c r="Z66" s="19">
+        <f t="shared" si="37"/>
+        <v>6.873971355534545</v>
+      </c>
+      <c r="AA66" s="19">
+        <f t="shared" si="37"/>
+        <v>17.858027618717308</v>
+      </c>
+      <c r="AB66" s="19">
+        <f t="shared" si="37"/>
+        <v>22.097135175588871</v>
+      </c>
+      <c r="AC66" s="19">
+        <f t="shared" si="37"/>
+        <v>24.394597701559782</v>
+      </c>
+      <c r="AD66" s="19">
+        <f t="shared" si="37"/>
+        <v>23.189118923642983</v>
+      </c>
+      <c r="AE66" s="19">
+        <f t="shared" si="37"/>
+        <v>25.441972152314502</v>
+      </c>
+      <c r="AF66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T66" s="23" t="e">
+      <c r="AG66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U66" s="23" t="e">
+      <c r="AH66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="V66" s="23" t="e">
+      <c r="AI66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="W66" s="23" t="e">
+      <c r="AJ66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X66" s="23" t="e">
+      <c r="AK66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y66" s="23" t="e">
+      <c r="AL66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z66" s="23">
-        <f t="shared" si="37"/>
-        <v>6.873971355534545</v>
-      </c>
-      <c r="AA66" s="23" t="e">
+      <c r="AM66" s="19" t="e">
         <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC66" s="23">
-        <f t="shared" si="37"/>
-        <v>24.394597701559782</v>
-      </c>
-      <c r="AD66" s="23">
-        <f t="shared" si="37"/>
-        <v>23.189118923642983</v>
-      </c>
-      <c r="AE66" s="23">
-        <f t="shared" si="37"/>
-        <v>25.441972152314502</v>
-      </c>
-      <c r="AF66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM66" s="23" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="67" spans="2:39" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="22" t="s">
+    </row>
+    <row r="67" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="19" t="s">
         <v>2012</v>
       </c>
-      <c r="Z67" s="23">
+      <c r="S67" s="19">
+        <v>349.85500000000002</v>
+      </c>
+      <c r="T67" s="19">
+        <v>325.10500000000002</v>
+      </c>
+      <c r="U67" s="19">
+        <v>322.58300000000003</v>
+      </c>
+      <c r="V67" s="19">
+        <v>321.43</v>
+      </c>
+      <c r="W67" s="19">
+        <v>315.58300000000003</v>
+      </c>
+      <c r="X67" s="19">
+        <v>305.48700000000002</v>
+      </c>
+      <c r="Y67" s="19">
+        <v>290.315</v>
+      </c>
+      <c r="Z67" s="19">
         <v>285.57</v>
       </c>
-      <c r="AC67" s="23">
+      <c r="AA67" s="19">
+        <v>282.56200000000001</v>
+      </c>
+      <c r="AB67" s="19">
+        <v>281.93700000000001</v>
+      </c>
+      <c r="AC67" s="19">
         <v>280.10300000000001</v>
       </c>
-      <c r="AD67" s="23">
+      <c r="AD67" s="19">
         <v>272.32600000000002</v>
       </c>
-      <c r="AE67" s="23">
+      <c r="AE67" s="19">
         <v>225.297</v>
       </c>
     </row>
@@ -10388,8 +10560,8 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="71" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="20" t="s">
+    <row r="71" spans="2:39" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="18" t="s">
         <v>1968</v>
       </c>
     </row>
@@ -10722,8 +10894,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="20" t="s">
+    <row r="78" spans="2:39" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="18" t="s">
         <v>1969</v>
       </c>
     </row>
@@ -11048,109 +11220,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:39" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="26" t="s">
+    <row r="85" spans="2:39" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="21" t="s">
         <v>1096</v>
       </c>
-      <c r="P85" s="26">
+      <c r="P85" s="21">
         <f>P84+P77</f>
         <v>0</v>
       </c>
-      <c r="Q85" s="26">
+      <c r="Q85" s="21">
         <f t="shared" ref="Q85:AM85" si="40">Q84+Q77</f>
         <v>0</v>
       </c>
-      <c r="R85" s="26">
+      <c r="R85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="S85" s="26">
+      <c r="S85" s="21">
         <f t="shared" si="40"/>
         <v>35113</v>
       </c>
-      <c r="T85" s="26">
+      <c r="T85" s="21">
         <f t="shared" si="40"/>
         <v>37908</v>
       </c>
-      <c r="U85" s="26">
+      <c r="U85" s="21">
         <f t="shared" si="40"/>
         <v>38657</v>
       </c>
-      <c r="V85" s="26">
+      <c r="V85" s="21">
         <f t="shared" si="40"/>
         <v>36188</v>
       </c>
-      <c r="W85" s="26">
+      <c r="W85" s="21">
         <f t="shared" si="40"/>
         <v>37046</v>
       </c>
-      <c r="X85" s="26">
+      <c r="X85" s="21">
         <f t="shared" si="40"/>
         <v>49128</v>
       </c>
-      <c r="Y85" s="26">
+      <c r="Y85" s="21">
         <f t="shared" si="40"/>
         <v>47806</v>
       </c>
-      <c r="Z85" s="26">
+      <c r="Z85" s="21">
         <f t="shared" si="40"/>
         <v>46521</v>
       </c>
-      <c r="AA85" s="26">
+      <c r="AA85" s="21">
         <f t="shared" si="40"/>
         <v>44876</v>
       </c>
-      <c r="AB85" s="26">
+      <c r="AB85" s="21">
         <f t="shared" si="40"/>
         <v>47528</v>
       </c>
-      <c r="AC85" s="26">
+      <c r="AC85" s="21">
         <f t="shared" si="40"/>
         <v>50710</v>
       </c>
-      <c r="AD85" s="26">
+      <c r="AD85" s="21">
         <f t="shared" si="40"/>
         <v>50873</v>
       </c>
-      <c r="AE85" s="26">
+      <c r="AE85" s="21">
         <f t="shared" si="40"/>
         <v>52880</v>
       </c>
-      <c r="AF85" s="26">
+      <c r="AF85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AG85" s="26">
+      <c r="AG85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AH85" s="26">
+      <c r="AH85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AI85" s="26">
+      <c r="AI85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AJ85" s="26">
+      <c r="AJ85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AK85" s="26">
+      <c r="AK85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AL85" s="26">
+      <c r="AL85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AM85" s="26">
+      <c r="AM85" s="21">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="20" t="s">
+    <row r="86" spans="2:39" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="18" t="s">
         <v>1970</v>
       </c>
     </row>
@@ -11476,8 +11648,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="20" t="s">
+    <row r="93" spans="2:39" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="18" t="s">
         <v>1971</v>
       </c>
     </row>
@@ -11723,109 +11895,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:39" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="26" t="s">
+    <row r="98" spans="2:39" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="21" t="s">
         <v>1306</v>
       </c>
-      <c r="P98" s="26">
+      <c r="P98" s="21">
         <f>P97+P92</f>
         <v>0</v>
       </c>
-      <c r="Q98" s="26">
+      <c r="Q98" s="21">
         <f t="shared" ref="Q98:AM98" si="43">Q97+Q92</f>
         <v>0</v>
       </c>
-      <c r="R98" s="26">
+      <c r="R98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="S98" s="26">
+      <c r="S98" s="21">
         <f t="shared" si="43"/>
         <v>31616</v>
       </c>
-      <c r="T98" s="26">
+      <c r="T98" s="21">
         <f t="shared" si="43"/>
         <v>36907</v>
       </c>
-      <c r="U98" s="26">
+      <c r="U98" s="21">
         <f t="shared" si="43"/>
         <v>38618</v>
       </c>
-      <c r="V98" s="26">
+      <c r="V98" s="21">
         <f t="shared" si="43"/>
         <v>31270</v>
       </c>
-      <c r="W98" s="26">
+      <c r="W98" s="21">
         <f t="shared" si="43"/>
         <v>33646</v>
       </c>
-      <c r="X98" s="26">
+      <c r="X98" s="21">
         <f t="shared" si="43"/>
         <v>46031</v>
       </c>
-      <c r="Y98" s="26">
+      <c r="Y98" s="21">
         <f t="shared" si="43"/>
         <v>46200</v>
       </c>
-      <c r="Z98" s="26">
+      <c r="Z98" s="21">
         <f t="shared" si="43"/>
         <v>47130</v>
       </c>
-      <c r="AA98" s="26">
+      <c r="AA98" s="21">
         <f t="shared" si="43"/>
         <v>43427</v>
       </c>
-      <c r="AB98" s="26">
+      <c r="AB98" s="21">
         <f t="shared" si="43"/>
         <v>44357</v>
       </c>
-      <c r="AC98" s="26">
+      <c r="AC98" s="21">
         <f t="shared" si="43"/>
         <v>44672</v>
       </c>
-      <c r="AD98" s="26">
+      <c r="AD98" s="21">
         <f t="shared" si="43"/>
         <v>39914</v>
       </c>
-      <c r="AE98" s="26">
+      <c r="AE98" s="21">
         <f t="shared" si="43"/>
         <v>43614</v>
       </c>
-      <c r="AF98" s="26">
+      <c r="AF98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AG98" s="26">
+      <c r="AG98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AH98" s="26">
+      <c r="AH98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AI98" s="26">
+      <c r="AI98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AJ98" s="26">
+      <c r="AJ98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AK98" s="26">
+      <c r="AK98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AL98" s="26">
+      <c r="AL98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AM98" s="26">
+      <c r="AM98" s="21">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="20" t="s">
+    <row r="99" spans="2:39" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="18" t="s">
         <v>1972</v>
       </c>
     </row>
@@ -11961,47 +12133,47 @@
         <v>16943</v>
       </c>
     </row>
-    <row r="103" spans="2:39" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="24" t="s">
+    <row r="103" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="8" t="s">
         <v>2034</v>
       </c>
-      <c r="S103" s="24">
+      <c r="S103" s="8">
         <v>-9010</v>
       </c>
-      <c r="T103" s="24">
+      <c r="T103" s="8">
         <v>-11257</v>
       </c>
-      <c r="U103" s="24">
+      <c r="U103" s="8">
         <v>-13493</v>
       </c>
-      <c r="V103" s="24">
+      <c r="V103" s="8">
         <v>-9601</v>
       </c>
-      <c r="W103" s="24">
+      <c r="W103" s="8">
         <v>-11870</v>
       </c>
-      <c r="X103" s="24">
+      <c r="X103" s="8">
         <v>-11444</v>
       </c>
-      <c r="Y103" s="24">
+      <c r="Y103" s="8">
         <v>-12102</v>
       </c>
-      <c r="Z103" s="24">
+      <c r="Z103" s="8">
         <v>-12540</v>
       </c>
-      <c r="AA103" s="24">
+      <c r="AA103" s="8">
         <v>-14321</v>
       </c>
-      <c r="AB103" s="24">
+      <c r="AB103" s="8">
         <v>-15554</v>
       </c>
-      <c r="AC103" s="24">
+      <c r="AC103" s="8">
         <v>-16121</v>
       </c>
-      <c r="AD103" s="24">
+      <c r="AD103" s="8">
         <v>-11006</v>
       </c>
-      <c r="AE103" s="24">
+      <c r="AE103" s="8">
         <v>-8023</v>
       </c>
     </row>
@@ -12049,205 +12221,205 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:39" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="25" t="s">
+    <row r="105" spans="2:39" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="20" t="s">
         <v>2035</v>
       </c>
-      <c r="P105" s="25">
+      <c r="P105" s="20">
         <f>SUM(P100:P103)</f>
         <v>0</v>
       </c>
-      <c r="Q105" s="25">
+      <c r="Q105" s="20">
         <f t="shared" ref="Q105:AM105" si="44">SUM(Q100:Q103)</f>
         <v>0</v>
       </c>
-      <c r="R105" s="25">
+      <c r="R105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="S105" s="25">
-        <f>SUM(S100:S104)</f>
+      <c r="S105" s="20">
+        <f t="shared" ref="S105:AE105" si="45">SUM(S100:S104)</f>
         <v>3497</v>
       </c>
-      <c r="T105" s="25">
-        <f>SUM(T100:T104)</f>
+      <c r="T105" s="20">
+        <f t="shared" si="45"/>
         <v>1001</v>
       </c>
-      <c r="U105" s="25">
-        <f>SUM(U100:U104)</f>
+      <c r="U105" s="20">
+        <f t="shared" si="45"/>
         <v>39</v>
       </c>
-      <c r="V105" s="25">
-        <f>SUM(V100:V104)</f>
+      <c r="V105" s="20">
+        <f t="shared" si="45"/>
         <v>4918</v>
       </c>
-      <c r="W105" s="25">
-        <f>SUM(W100:W104)</f>
+      <c r="W105" s="20">
+        <f t="shared" si="45"/>
         <v>3400</v>
       </c>
-      <c r="X105" s="25">
-        <f>SUM(X100:X104)</f>
+      <c r="X105" s="20">
+        <f t="shared" si="45"/>
         <v>3097</v>
       </c>
-      <c r="Y105" s="25">
-        <f>SUM(Y100:Y104)</f>
+      <c r="Y105" s="20">
+        <f t="shared" si="45"/>
         <v>1606</v>
       </c>
-      <c r="Z105" s="25">
-        <f>SUM(Z100:Z104)</f>
+      <c r="Z105" s="20">
+        <f t="shared" si="45"/>
         <v>-609</v>
       </c>
-      <c r="AA105" s="25">
-        <f>SUM(AA100:AA104)</f>
+      <c r="AA105" s="20">
+        <f t="shared" si="45"/>
         <v>1449</v>
       </c>
-      <c r="AB105" s="25">
-        <f>SUM(AB100:AB104)</f>
+      <c r="AB105" s="20">
+        <f t="shared" si="45"/>
         <v>3171</v>
       </c>
-      <c r="AC105" s="25">
-        <f>SUM(AC100:AC104)</f>
+      <c r="AC105" s="20">
+        <f t="shared" si="45"/>
         <v>6038</v>
       </c>
-      <c r="AD105" s="25">
-        <f>SUM(AD100:AD104)</f>
+      <c r="AD105" s="20">
+        <f t="shared" si="45"/>
         <v>10959</v>
       </c>
-      <c r="AE105" s="25">
-        <f>SUM(AE100:AE104)</f>
+      <c r="AE105" s="20">
+        <f t="shared" si="45"/>
         <v>9266</v>
       </c>
-      <c r="AF105" s="25">
+      <c r="AF105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AG105" s="25">
+      <c r="AG105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AH105" s="25">
+      <c r="AH105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AI105" s="25">
+      <c r="AI105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AJ105" s="25">
+      <c r="AJ105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AK105" s="25">
+      <c r="AK105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AL105" s="25">
+      <c r="AL105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AM105" s="25">
+      <c r="AM105" s="20">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:39" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="26" t="s">
+    <row r="106" spans="2:39" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="21" t="s">
         <v>2036</v>
       </c>
-      <c r="P106" s="26">
+      <c r="P106" s="21">
         <f>P105+P98</f>
         <v>0</v>
       </c>
-      <c r="Q106" s="26">
-        <f t="shared" ref="Q106:AM106" si="45">Q105+Q98</f>
-        <v>0</v>
-      </c>
-      <c r="R106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S106" s="26">
-        <f t="shared" si="45"/>
+      <c r="Q106" s="21">
+        <f t="shared" ref="Q106:AM106" si="46">Q105+Q98</f>
+        <v>0</v>
+      </c>
+      <c r="R106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S106" s="21">
+        <f t="shared" si="46"/>
         <v>35113</v>
       </c>
-      <c r="T106" s="26">
-        <f t="shared" si="45"/>
+      <c r="T106" s="21">
+        <f t="shared" si="46"/>
         <v>37908</v>
       </c>
-      <c r="U106" s="26">
-        <f t="shared" si="45"/>
+      <c r="U106" s="21">
+        <f t="shared" si="46"/>
         <v>38657</v>
       </c>
-      <c r="V106" s="26">
-        <f t="shared" si="45"/>
+      <c r="V106" s="21">
+        <f t="shared" si="46"/>
         <v>36188</v>
       </c>
-      <c r="W106" s="26">
-        <f t="shared" si="45"/>
+      <c r="W106" s="21">
+        <f t="shared" si="46"/>
         <v>37046</v>
       </c>
-      <c r="X106" s="26">
-        <f t="shared" si="45"/>
+      <c r="X106" s="21">
+        <f t="shared" si="46"/>
         <v>49128</v>
       </c>
-      <c r="Y106" s="26">
-        <f t="shared" si="45"/>
+      <c r="Y106" s="21">
+        <f t="shared" si="46"/>
         <v>47806</v>
       </c>
-      <c r="Z106" s="26">
-        <f t="shared" si="45"/>
+      <c r="Z106" s="21">
+        <f t="shared" si="46"/>
         <v>46521</v>
       </c>
-      <c r="AA106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AA106" s="21">
+        <f t="shared" si="46"/>
         <v>44876</v>
       </c>
-      <c r="AB106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AB106" s="21">
+        <f t="shared" si="46"/>
         <v>47528</v>
       </c>
-      <c r="AC106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AC106" s="21">
+        <f t="shared" si="46"/>
         <v>50710</v>
       </c>
-      <c r="AD106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AD106" s="21">
+        <f t="shared" si="46"/>
         <v>50873</v>
       </c>
-      <c r="AE106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AE106" s="21">
+        <f t="shared" si="46"/>
         <v>52880</v>
       </c>
-      <c r="AF106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AG106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AH106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AI106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AJ106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AK106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AL106" s="26">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="AM106" s="26">
-        <f t="shared" si="45"/>
+      <c r="AF106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AG106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AH106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AI106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AJ106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AK106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AL106" s="21">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AM106" s="21">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
@@ -12353,95 +12525,95 @@
         <v>0</v>
       </c>
       <c r="Q110" s="8">
-        <f t="shared" ref="Q110:AM110" si="46">SUM(Q108:Q109)</f>
+        <f t="shared" ref="Q110:AM110" si="47">SUM(Q108:Q109)</f>
         <v>0</v>
       </c>
       <c r="R110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="S110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>2981</v>
       </c>
       <c r="T110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>3266</v>
       </c>
       <c r="U110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>619</v>
       </c>
       <c r="V110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>3710</v>
       </c>
       <c r="W110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>3021</v>
       </c>
       <c r="X110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>4162</v>
       </c>
       <c r="Y110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>4126</v>
       </c>
       <c r="Z110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>5299</v>
       </c>
       <c r="AA110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1860</v>
       </c>
       <c r="AB110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>5827</v>
       </c>
       <c r="AC110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>6417</v>
       </c>
       <c r="AD110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>7699</v>
       </c>
       <c r="AE110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>6132</v>
       </c>
       <c r="AF110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AG110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AH110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AI110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AJ110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AK110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AL110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AM110" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
     </row>
@@ -12631,15 +12803,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q116" s="12" t="e">
-        <f t="shared" ref="Q116:S116" si="47">ABS(Q115)/Q64</f>
+        <f t="shared" ref="Q116:S116" si="48">ABS(Q115)/Q64</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R116" s="12" t="e">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S116" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.3366921473245309</v>
       </c>
       <c r="T116" s="12">
@@ -12647,94 +12819,894 @@
         <v>0.41242937853107342</v>
       </c>
       <c r="U116" s="12">
-        <f t="shared" ref="U116:AM116" si="48">ABS(U115)/U64</f>
+        <f t="shared" ref="U116:AM116" si="49">ABS(U115)/U64</f>
         <v>0.49253187613843352</v>
       </c>
       <c r="V116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.51660516605166051</v>
       </c>
       <c r="W116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.4869950193691201</v>
       </c>
       <c r="X116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.53592233009708734</v>
       </c>
       <c r="Y116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.39590179779624973</v>
       </c>
       <c r="Z116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1.1018848700967907</v>
       </c>
       <c r="AA116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.46512088783194611</v>
       </c>
       <c r="AB116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.41027287319422151</v>
       </c>
       <c r="AC116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.40450753695302211</v>
       </c>
       <c r="AD116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.46555819477434679</v>
       </c>
       <c r="AE116" s="12">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0.526168876482903</v>
       </c>
       <c r="AF116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AL116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AM116" s="12" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="117" spans="2:39" s="14" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="118" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="119" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="120" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="121" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" spans="2:39" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="14" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="118" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="8" t="s">
+        <v>2050</v>
+      </c>
+      <c r="S118" s="8">
+        <f>S9*S119</f>
+        <v>23678.186400000002</v>
+      </c>
+      <c r="T118" s="8">
+        <f t="shared" ref="T118:AM118" si="50">T9*T119</f>
+        <v>21573.967800000002</v>
+      </c>
+      <c r="U118" s="8">
+        <f t="shared" si="50"/>
+        <v>25500.186150000001</v>
+      </c>
+      <c r="V118" s="8">
+        <f t="shared" si="50"/>
+        <v>27604.4084</v>
+      </c>
+      <c r="W118" s="8">
+        <f t="shared" si="50"/>
+        <v>45661.704270000002</v>
+      </c>
+      <c r="X118" s="8">
+        <f t="shared" si="50"/>
+        <v>55571.140170000006</v>
+      </c>
+      <c r="Y118" s="8">
+        <f t="shared" si="50"/>
+        <v>58199.448049999999</v>
+      </c>
+      <c r="Z118" s="8">
+        <f t="shared" si="50"/>
+        <v>69701.925600000002</v>
+      </c>
+      <c r="AA118" s="8">
+        <f t="shared" si="50"/>
+        <v>79111.708760000009</v>
+      </c>
+      <c r="AB118" s="8">
+        <f t="shared" si="50"/>
+        <v>87473.773620000007</v>
+      </c>
+      <c r="AC118" s="8">
+        <f t="shared" si="50"/>
+        <v>97352.59868000001</v>
+      </c>
+      <c r="AD118" s="8">
+        <f t="shared" si="50"/>
+        <v>91896.4087</v>
+      </c>
+      <c r="AE118" s="8">
+        <f t="shared" si="50"/>
+        <v>94113.31581</v>
+      </c>
+      <c r="AF118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AG118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AH118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AI118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AJ118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AK118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AL118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AM118" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S119" s="8">
+        <f>S67</f>
+        <v>349.85500000000002</v>
+      </c>
+      <c r="T119" s="8">
+        <f t="shared" ref="T119:AM119" si="51">T67</f>
+        <v>325.10500000000002</v>
+      </c>
+      <c r="U119" s="8">
+        <f t="shared" si="51"/>
+        <v>322.58300000000003</v>
+      </c>
+      <c r="V119" s="8">
+        <f t="shared" si="51"/>
+        <v>321.43</v>
+      </c>
+      <c r="W119" s="8">
+        <f t="shared" si="51"/>
+        <v>315.58300000000003</v>
+      </c>
+      <c r="X119" s="8">
+        <f t="shared" si="51"/>
+        <v>305.48700000000002</v>
+      </c>
+      <c r="Y119" s="8">
+        <f t="shared" si="51"/>
+        <v>290.315</v>
+      </c>
+      <c r="Z119" s="8">
+        <f t="shared" si="51"/>
+        <v>285.57</v>
+      </c>
+      <c r="AA119" s="8">
+        <f t="shared" si="51"/>
+        <v>282.56200000000001</v>
+      </c>
+      <c r="AB119" s="8">
+        <f t="shared" si="51"/>
+        <v>281.93700000000001</v>
+      </c>
+      <c r="AC119" s="8">
+        <f t="shared" si="51"/>
+        <v>280.10300000000001</v>
+      </c>
+      <c r="AD119" s="8">
+        <f t="shared" si="51"/>
+        <v>272.32600000000002</v>
+      </c>
+      <c r="AE119" s="8">
+        <f t="shared" si="51"/>
+        <v>225.297</v>
+      </c>
+      <c r="AF119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AG119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AH119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AI119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AJ119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AK119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AL119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="AM119" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B120" s="19" t="s">
+        <v>2051</v>
+      </c>
+      <c r="S120" s="19">
+        <f>S118/S43</f>
+        <v>0.51845123601410092</v>
+      </c>
+      <c r="T120" s="19">
+        <f t="shared" ref="T120:AM120" si="52">T118/T43</f>
+        <v>0.46396627454353861</v>
+      </c>
+      <c r="U120" s="19">
+        <f t="shared" si="52"/>
+        <v>0.54046429040735877</v>
+      </c>
+      <c r="V120" s="19">
+        <f t="shared" si="52"/>
+        <v>0.60858962917236215</v>
+      </c>
+      <c r="W120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.0013531638157895</v>
+      </c>
+      <c r="X120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.2046115531518253</v>
+      </c>
+      <c r="Y120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.230692494184817</v>
+      </c>
+      <c r="Z120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.3951546357085669</v>
+      </c>
+      <c r="AA120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.4715172195974853</v>
+      </c>
+      <c r="AB120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.4624786601350901</v>
+      </c>
+      <c r="AC120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.4886173687268724</v>
+      </c>
+      <c r="AD120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.3706880362150229</v>
+      </c>
+      <c r="AE120" s="19">
+        <f t="shared" si="52"/>
+        <v>1.4263051013882153</v>
+      </c>
+      <c r="AF120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM120" s="19" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="19" t="s">
+        <v>2052</v>
+      </c>
+      <c r="S121" s="19">
+        <f>S118/S64</f>
+        <v>8.2273059068797778</v>
+      </c>
+      <c r="T121" s="19">
+        <f t="shared" ref="T121:AM121" si="53">T118/T64</f>
+        <v>8.1257882485875719</v>
+      </c>
+      <c r="U121" s="19">
+        <f t="shared" si="53"/>
+        <v>9.2896853005464486</v>
+      </c>
+      <c r="V121" s="19">
+        <f t="shared" si="53"/>
+        <v>9.2601168735323718</v>
+      </c>
+      <c r="W121" s="19">
+        <f t="shared" si="53"/>
+        <v>12.634671906474821</v>
+      </c>
+      <c r="X121" s="19">
+        <f t="shared" si="53"/>
+        <v>15.415018077669904</v>
+      </c>
+      <c r="Y121" s="19">
+        <f t="shared" si="53"/>
+        <v>11.250618219601778</v>
+      </c>
+      <c r="Z121" s="19">
+        <f t="shared" si="53"/>
+        <v>35.507858176260825</v>
+      </c>
+      <c r="AA121" s="19">
+        <f t="shared" si="53"/>
+        <v>15.678103202536665</v>
+      </c>
+      <c r="AB121" s="19">
+        <f t="shared" si="53"/>
+        <v>14.040734128410916</v>
+      </c>
+      <c r="AC121" s="19">
+        <f t="shared" si="53"/>
+        <v>14.247416753988</v>
+      </c>
+      <c r="AD121" s="19">
+        <f t="shared" si="53"/>
+        <v>14.552083721298496</v>
+      </c>
+      <c r="AE121" s="19">
+        <f t="shared" si="53"/>
+        <v>16.418931578855549</v>
+      </c>
+      <c r="AF121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM121" s="19" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B122" s="19" t="s">
+        <v>2053</v>
+      </c>
+      <c r="S122" s="19">
+        <f>S118/S105</f>
+        <v>6.7709998284243644</v>
+      </c>
+      <c r="T122" s="19">
+        <f t="shared" ref="T122:AM122" si="54">T118/T105</f>
+        <v>21.552415384615387</v>
+      </c>
+      <c r="U122" s="19">
+        <f t="shared" si="54"/>
+        <v>653.85092692307694</v>
+      </c>
+      <c r="V122" s="19">
+        <f t="shared" si="54"/>
+        <v>5.6129337942252953</v>
+      </c>
+      <c r="W122" s="19">
+        <f t="shared" si="54"/>
+        <v>13.429913020588236</v>
+      </c>
+      <c r="X122" s="19">
+        <f t="shared" si="54"/>
+        <v>17.943538963513078</v>
+      </c>
+      <c r="Y122" s="19">
+        <f t="shared" si="54"/>
+        <v>36.238759682440843</v>
+      </c>
+      <c r="Z122" s="19">
+        <f t="shared" si="54"/>
+        <v>-114.45307980295567</v>
+      </c>
+      <c r="AA122" s="19">
+        <f t="shared" si="54"/>
+        <v>54.597452560386479</v>
+      </c>
+      <c r="AB122" s="19">
+        <f t="shared" si="54"/>
+        <v>27.585548287606436</v>
+      </c>
+      <c r="AC122" s="19">
+        <f t="shared" si="54"/>
+        <v>16.123318761179199</v>
+      </c>
+      <c r="AD122" s="19">
+        <f t="shared" si="54"/>
+        <v>8.3854739209781908</v>
+      </c>
+      <c r="AE122" s="19">
+        <f t="shared" si="54"/>
+        <v>10.156843925102525</v>
+      </c>
+      <c r="AF122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM122" s="19" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="2:39" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B123" s="19" t="s">
+        <v>2054</v>
+      </c>
+      <c r="S123" s="19">
+        <f>S118/S110</f>
+        <v>7.9430346863468646</v>
+      </c>
+      <c r="T123" s="19">
+        <f t="shared" ref="T123:AM123" si="55">T118/T110</f>
+        <v>6.6056239436619721</v>
+      </c>
+      <c r="U123" s="19">
+        <f t="shared" si="55"/>
+        <v>41.195777302100161</v>
+      </c>
+      <c r="V123" s="19">
+        <f t="shared" si="55"/>
+        <v>7.4405413477088951</v>
+      </c>
+      <c r="W123" s="19">
+        <f t="shared" si="55"/>
+        <v>15.114764736842107</v>
+      </c>
+      <c r="X123" s="19">
+        <f t="shared" si="55"/>
+        <v>13.35202791206151</v>
+      </c>
+      <c r="Y123" s="19">
+        <f t="shared" si="55"/>
+        <v>14.105537578768782</v>
+      </c>
+      <c r="Z123" s="19">
+        <f t="shared" si="55"/>
+        <v>13.153788563879978</v>
+      </c>
+      <c r="AA123" s="19">
+        <f t="shared" si="55"/>
+        <v>42.533176752688178</v>
+      </c>
+      <c r="AB123" s="19">
+        <f t="shared" si="55"/>
+        <v>15.011802577655741</v>
+      </c>
+      <c r="AC123" s="19">
+        <f t="shared" si="55"/>
+        <v>15.171045454262117</v>
+      </c>
+      <c r="AD123" s="19">
+        <f t="shared" si="55"/>
+        <v>11.936148681646968</v>
+      </c>
+      <c r="AE123" s="19">
+        <f t="shared" si="55"/>
+        <v>15.347898860078278</v>
+      </c>
+      <c r="AF123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM123" s="19" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="124" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="125" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="126" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="127" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="128" spans="2:39" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="2:39" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B125" s="16" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="126" spans="2:39" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B126" s="22" t="s">
+        <v>2056</v>
+      </c>
+      <c r="S126" s="22" t="e">
+        <f>(S43-R43)/ABS(R43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T126" s="22">
+        <f t="shared" ref="T126:AM126" si="56">(T43-S43)/ABS(S43)</f>
+        <v>1.8129666527993693E-2</v>
+      </c>
+      <c r="U126" s="22">
+        <f t="shared" si="56"/>
+        <v>1.4688487924471494E-2</v>
+      </c>
+      <c r="V126" s="22">
+        <f t="shared" si="56"/>
+        <v>-3.8658810563350431E-2</v>
+      </c>
+      <c r="W126" s="22">
+        <f t="shared" si="56"/>
+        <v>5.3353322456898451E-3</v>
+      </c>
+      <c r="X126" s="22">
+        <f t="shared" si="56"/>
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="Y126" s="22">
+        <f t="shared" si="56"/>
+        <v>2.5101881557270441E-2</v>
+      </c>
+      <c r="Z126" s="22">
+        <f t="shared" si="56"/>
+        <v>5.6460139564389937E-2</v>
+      </c>
+      <c r="AA126" s="22">
+        <f t="shared" si="56"/>
+        <v>7.6100880704563653E-2</v>
+      </c>
+      <c r="AB126" s="22">
+        <f t="shared" si="56"/>
+        <v>0.11253301588482571</v>
+      </c>
+      <c r="AC126" s="22">
+        <f t="shared" si="56"/>
+        <v>9.3392630241423122E-2</v>
+      </c>
+      <c r="AD126" s="22">
+        <f t="shared" si="56"/>
+        <v>2.5168965411786294E-2</v>
+      </c>
+      <c r="AE126" s="22">
+        <f t="shared" si="56"/>
+        <v>-1.581051249925422E-2</v>
+      </c>
+      <c r="AF126" s="22">
+        <f t="shared" si="56"/>
+        <v>-1</v>
+      </c>
+      <c r="AG126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM126" s="22" t="e">
+        <f t="shared" si="56"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="2:39" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B127" s="22" t="s">
+        <v>2057</v>
+      </c>
+      <c r="S127" s="22" t="e">
+        <f>(S64-R64)/ABS(R64)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T127" s="22">
+        <f t="shared" ref="T127:AM127" si="57">(T64-S64)/ABS(S64)</f>
+        <v>-7.7484364141765114E-2</v>
+      </c>
+      <c r="U127" s="22">
+        <f t="shared" si="57"/>
+        <v>3.3898305084745763E-2</v>
+      </c>
+      <c r="V127" s="22">
+        <f t="shared" si="57"/>
+        <v>8.5974499089253184E-2</v>
+      </c>
+      <c r="W127" s="22">
+        <f t="shared" si="57"/>
+        <v>0.21234485072123449</v>
+      </c>
+      <c r="X127" s="22">
+        <f t="shared" si="57"/>
+        <v>-2.4903154399557276E-3</v>
+      </c>
+      <c r="Y127" s="22">
+        <f t="shared" si="57"/>
+        <v>0.43495145631067961</v>
+      </c>
+      <c r="Z127" s="22">
+        <f t="shared" si="57"/>
+        <v>-0.62052967330369224</v>
+      </c>
+      <c r="AA127" s="22">
+        <f t="shared" si="57"/>
+        <v>1.5705552725420275</v>
+      </c>
+      <c r="AB127" s="22">
+        <f t="shared" si="57"/>
+        <v>0.23464130003963535</v>
+      </c>
+      <c r="AC127" s="22">
+        <f t="shared" si="57"/>
+        <v>9.678972712680578E-2</v>
+      </c>
+      <c r="AD127" s="22">
+        <f t="shared" si="57"/>
+        <v>-7.5808576028098928E-2</v>
+      </c>
+      <c r="AE127" s="22">
+        <f t="shared" si="57"/>
+        <v>-9.2319873317498025E-2</v>
+      </c>
+      <c r="AF127" s="22">
+        <f t="shared" si="57"/>
+        <v>-1</v>
+      </c>
+      <c r="AG127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM127" s="22" t="e">
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="2:39" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B128" s="22" t="s">
+        <v>2058</v>
+      </c>
+      <c r="S128" s="22" t="e">
+        <f>(S110-R110)/ABS(R110)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T128" s="22">
+        <f t="shared" ref="T128:AM128" si="58">(T110-S110)/ABS(S110)</f>
+        <v>9.5605501509560556E-2</v>
+      </c>
+      <c r="U128" s="22">
+        <f t="shared" si="58"/>
+        <v>-0.81047152480097984</v>
+      </c>
+      <c r="V128" s="22">
+        <f t="shared" si="58"/>
+        <v>4.9935379644588043</v>
+      </c>
+      <c r="W128" s="22">
+        <f t="shared" si="58"/>
+        <v>-0.18571428571428572</v>
+      </c>
+      <c r="X128" s="22">
+        <f t="shared" si="58"/>
+        <v>0.37768950678583252</v>
+      </c>
+      <c r="Y128" s="22">
+        <f t="shared" si="58"/>
+        <v>-8.649687650168188E-3</v>
+      </c>
+      <c r="Z128" s="22">
+        <f t="shared" si="58"/>
+        <v>0.28429471643238002</v>
+      </c>
+      <c r="AA128" s="22">
+        <f t="shared" si="58"/>
+        <v>-0.64899037554255523</v>
+      </c>
+      <c r="AB128" s="22">
+        <f t="shared" si="58"/>
+        <v>2.1327956989247312</v>
+      </c>
+      <c r="AC128" s="22">
+        <f t="shared" si="58"/>
+        <v>0.10125278874206281</v>
+      </c>
+      <c r="AD128" s="22">
+        <f t="shared" si="58"/>
+        <v>0.19978182951534984</v>
+      </c>
+      <c r="AE128" s="22">
+        <f t="shared" si="58"/>
+        <v>-0.20353292635407197</v>
+      </c>
+      <c r="AF128" s="22">
+        <f t="shared" si="58"/>
+        <v>-1</v>
+      </c>
+      <c r="AG128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM128" s="22" t="e">
+        <f t="shared" si="58"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="129" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="130" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>